<commit_message>
Updated BOM and schematic pdf
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
+++ b/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_DAC\REV20200627B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4116B7-BC3C-4793-A761-AA691D9264B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8B84D-F9A2-4151-A04C-474FE7D7A03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC92099F-4568-4F42-8FC0-039B72E8D4B9}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC_bom_qty_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">DAC_bom_qty_1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -138,16 +149,13 @@
     <t>S9337-ND</t>
   </si>
   <si>
-    <t>JMP1, JMP2, JMP3, JMP4, JMP5</t>
-  </si>
-  <si>
     <t>JMP_SHORT</t>
   </si>
   <si>
     <t>SAM8995-ND</t>
   </si>
   <si>
-    <t>JP1, JP2, JP3, JP4, JP5</t>
+    <t>JP1, JP2, JP3, JP4, JP5, JP6, JP7, JP8</t>
   </si>
   <si>
     <t>TSW-103-07-F-S</t>
@@ -207,7 +215,7 @@
     <t>P20086CT-ND</t>
   </si>
   <si>
-    <t>R6, R8, R14, R22, R24, R30, R32, R38</t>
+    <t>R6, R8, R14, R22, R24, R30, R32, R38, R39, R40, R41</t>
   </si>
   <si>
     <t>ERJ-PB3B1002V</t>
@@ -373,6 +381,9 @@
   </si>
   <si>
     <t>DAC60508MCRTET</t>
+  </si>
+  <si>
+    <t>JMP1, JMP2, JMP3, JMP4, JMP5, JMP6, JMP7, JMP8</t>
   </si>
 </sst>
 </file>
@@ -381,19 +392,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -402,25 +413,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -438,82 +436,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -521,7 +457,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -829,27 +765,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06187A11-79F7-461C-98CF-5964F459C446}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -868,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>8</v>
       </c>
@@ -884,641 +819,607 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="F2" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>8</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>4</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="B22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="B27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>8</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>8</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>8</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>4</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>4</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>1</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>1</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>2</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="B28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8">
+      <c r="C28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
-        <v>2</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="7" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>1</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="C32" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>1</v>
-      </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup orientation="landscape" blackAndWhite="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup orientation="landscape" blackAndWhite="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup orientation="landscape" blackAndWhite="1"/>
+  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
+  <pageSetup scale="62" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
R16 was old 1% tolerance resistor, updated to 0.1% tolerance resistor
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
+++ b/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_DAC\REV20200627B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8B84D-F9A2-4151-A04C-474FE7D7A03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5EA66D-6BF1-4564-9F12-2459CF6844EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC92099F-4568-4F42-8FC0-039B72E8D4B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC_bom_qty_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">DAC_bom_qty_1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Quantity</t>
   </si>
@@ -149,6 +138,9 @@
     <t>S9337-ND</t>
   </si>
   <si>
+    <t>JMP1, JMP2, JMP3, JMP4, JMP5, JMP6, JMP7, JMP8</t>
+  </si>
+  <si>
     <t>JMP_SHORT</t>
   </si>
   <si>
@@ -215,7 +207,7 @@
     <t>P20086CT-ND</t>
   </si>
   <si>
-    <t>R6, R8, R14, R22, R24, R30, R32, R38, R39, R40, R41</t>
+    <t>R6, R8, R14, R16, R22, R24, R30, R32, R38, R39, R40, R41</t>
   </si>
   <si>
     <t>ERJ-PB3B1002V</t>
@@ -248,15 +240,6 @@
     <t>30K</t>
   </si>
   <si>
-    <t>YAG2321CT-ND</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>RT0603FRE0710KL</t>
-  </si>
-  <si>
     <t>PTS647SK38SMTR2LFSCT-ND</t>
   </si>
   <si>
@@ -381,9 +364,6 @@
   </si>
   <si>
     <t>DAC60508MCRTET</t>
-  </si>
-  <si>
-    <t>JMP1, JMP2, JMP3, JMP4, JMP5, JMP6, JMP7, JMP8</t>
   </si>
 </sst>
 </file>
@@ -392,19 +372,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -413,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -422,6 +402,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -431,6 +424,54 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -438,18 +479,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -457,7 +512,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -765,26 +820,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06187A11-79F7-461C-98CF-5964F459C446}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -803,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>8</v>
       </c>
@@ -819,607 +874,621 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="F2" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="F4" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>5</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>4</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="E13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="3">
+      <c r="E14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="3">
+      <c r="E15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>11</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="E16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>12</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>8</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="E17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="F17" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>8</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>8</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="E18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="F18" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>8</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="F19" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="D21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8">
         <v>4</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="4" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3">
+      <c r="D22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>4</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="D23" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="D24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="D25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>2</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="D26" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8">
         <v>2</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="4" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>2</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3">
+      <c r="D27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>2</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="4" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="D28" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="E28" s="7"/>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="D29" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="E29" s="7"/>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="D30" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>1</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="D31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="E31" s="7"/>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>1</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="D32" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="E32" s="7"/>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>1</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="D33" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3">
+      <c r="E33" s="7"/>
+      <c r="F33" s="8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="62" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup orientation="landscape" blackAndWhite="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup orientation="landscape" blackAndWhite="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup orientation="landscape" blackAndWhite="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed DNP resistor and mounting holes from BOM
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
+++ b/Accessories/ExpansionBoard_DAC/REV20200627B/DAC_bom_qty_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_DAC\REV20200627B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5EA66D-6BF1-4564-9F12-2459CF6844EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD681237-C822-4164-AEA2-C2F595DED49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Quantity</t>
   </si>
@@ -151,21 +151,6 @@
   </si>
   <si>
     <t>TSW-103-07-F-S</t>
-  </si>
-  <si>
-    <t>MH1, MH2, MH3, MH4</t>
-  </si>
-  <si>
-    <t>MOUNT_HOLE</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>DNP</t>
   </si>
   <si>
     <t>311-2.80KHRCT-ND</t>
@@ -824,10 +809,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1052,328 +1037,334 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="C13" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="F13" s="8">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F14" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F15" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F16" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F17" s="8">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>1</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8">
@@ -1385,13 +1376,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="8">
@@ -1403,52 +1394,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>1</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8">
         <v>1</v>
       </c>
     </row>

</xml_diff>